<commit_message>
pobiera rowniez zdjecia profilowe
</commit_message>
<xml_diff>
--- a/animals.xlsx
+++ b/animals.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="237">
   <si>
     <t>Imię</t>
   </si>
@@ -33,6 +33,9 @@
     <t>Rozmiar</t>
   </si>
   <si>
+    <t>URL zdjęcia</t>
+  </si>
+  <si>
     <t>Ariel</t>
   </si>
   <si>
@@ -45,6 +48,9 @@
     <t>średni (17kg)</t>
   </si>
   <si>
+    <t>https://schroniskochorzow.pl/wp-content/uploads/2024/06/58793A.png</t>
+  </si>
+  <si>
     <t>Atena</t>
   </si>
   <si>
@@ -54,6 +60,9 @@
     <t>średni (20kg)</t>
   </si>
   <si>
+    <t>https://schroniskochorzow.pl/wp-content/uploads/2024/07/Atena-29619.png</t>
+  </si>
+  <si>
     <t>Bastek</t>
   </si>
   <si>
@@ -66,6 +75,9 @@
     <t>duży (32kg)</t>
   </si>
   <si>
+    <t>https://schroniskochorzow.pl/wp-content/uploads/2024/07/bastek-2.png</t>
+  </si>
+  <si>
     <t>Batman</t>
   </si>
   <si>
@@ -78,6 +90,9 @@
     <t>mały (11kg)</t>
   </si>
   <si>
+    <t>https://schroniskochorzow.pl/wp-content/uploads/2024/07/227-Batman.png</t>
+  </si>
+  <si>
     <t>Dziadek</t>
   </si>
   <si>
@@ -90,6 +105,9 @@
     <t>mały (9kg)</t>
   </si>
   <si>
+    <t>https://schroniskochorzow.pl/wp-content/uploads/2024/07/274-Dziadek.png</t>
+  </si>
+  <si>
     <t>Eboni</t>
   </si>
   <si>
@@ -99,6 +117,9 @@
     <t>mały (5kg)</t>
   </si>
   <si>
+    <t>https://schroniskochorzow.pl/wp-content/uploads/2024/07/270-EBONI.png</t>
+  </si>
+  <si>
     <t>Elvis</t>
   </si>
   <si>
@@ -108,6 +129,9 @@
     <t>średni (13,5kg)</t>
   </si>
   <si>
+    <t>https://schroniskochorzow.pl/wp-content/uploads/2024/07/297-Elvis.png</t>
+  </si>
+  <si>
     <t>Fistaszek i Orzeszek</t>
   </si>
   <si>
@@ -123,24 +147,36 @@
     <t>mały (7kg)</t>
   </si>
   <si>
+    <t>https://schroniskochorzow.pl/wp-content/uploads/2024/06/orzeszek-fistaszek.png</t>
+  </si>
+  <si>
     <t>Gordon</t>
   </si>
   <si>
     <t>duży (30 kg)</t>
   </si>
   <si>
+    <t>https://schroniskochorzow.pl/wp-content/uploads/2024/07/43414-GORDON-1.png</t>
+  </si>
+  <si>
     <t>Heidi</t>
   </si>
   <si>
     <t>duży (30kg)</t>
   </si>
   <si>
+    <t>https://schroniskochorzow.pl/wp-content/uploads/2024/07/78878.png</t>
+  </si>
+  <si>
     <t>Idea</t>
   </si>
   <si>
     <t>duży (27kg)</t>
   </si>
   <si>
+    <t>https://schroniskochorzow.pl/wp-content/uploads/2024/07/34743.png</t>
+  </si>
+  <si>
     <t>Kara</t>
   </si>
   <si>
@@ -150,6 +186,9 @@
     <t>duży (31kg)</t>
   </si>
   <si>
+    <t>https://schroniskochorzow.pl/wp-content/uploads/2024/07/kara-2.png</t>
+  </si>
+  <si>
     <t>King</t>
   </si>
   <si>
@@ -159,6 +198,9 @@
     <t>olbrzymi (51kg)</t>
   </si>
   <si>
+    <t>https://schroniskochorzow.pl/wp-content/uploads/2024/06/king1.png</t>
+  </si>
+  <si>
     <t>Lipka</t>
   </si>
   <si>
@@ -171,6 +213,9 @@
     <t>mały (12kg) – docelowo średni/duży</t>
   </si>
   <si>
+    <t>https://schroniskochorzow.pl/wp-content/uploads/2024/07/291-LIPKA.png</t>
+  </si>
+  <si>
     <t>Marley</t>
   </si>
   <si>
@@ -180,6 +225,9 @@
     <t>duży (40 kg)</t>
   </si>
   <si>
+    <t>https://schroniskochorzow.pl/wp-content/uploads/2024/07/12822-Marley.png</t>
+  </si>
+  <si>
     <t>Mars</t>
   </si>
   <si>
@@ -192,33 +240,51 @@
     <t>duży (26 kg)</t>
   </si>
   <si>
+    <t>https://schroniskochorzow.pl/wp-content/uploads/2024/06/251-MARS.png</t>
+  </si>
+  <si>
     <t>Marvel</t>
   </si>
   <si>
+    <t>https://schroniskochorzow.pl/wp-content/uploads/2024/07/marvel-7.png</t>
+  </si>
+  <si>
     <t>Melonik</t>
   </si>
   <si>
     <t>średni (25kg)</t>
   </si>
   <si>
+    <t>https://schroniskochorzow.pl/wp-content/uploads/2024/06/melonik.png</t>
+  </si>
+  <si>
     <t>Miron</t>
   </si>
   <si>
     <t>duży (34 kg)</t>
   </si>
   <si>
+    <t>https://schroniskochorzow.pl/wp-content/uploads/2024/07/miron-1.png</t>
+  </si>
+  <si>
     <t>Mniszek</t>
   </si>
   <si>
     <t>średni (14kg)</t>
   </si>
   <si>
+    <t>https://schroniskochorzow.pl/wp-content/uploads/2024/06/mniszek.png</t>
+  </si>
+  <si>
     <t>Negro</t>
   </si>
   <si>
     <t>269/24</t>
   </si>
   <si>
+    <t>https://schroniskochorzow.pl/wp-content/uploads/2024/07/269.png</t>
+  </si>
+  <si>
     <t>Norek</t>
   </si>
   <si>
@@ -231,12 +297,18 @@
     <t>mały (12 kg)</t>
   </si>
   <si>
+    <t>https://schroniskochorzow.pl/wp-content/uploads/2024/06/245-NOREK.png</t>
+  </si>
+  <si>
     <t>Pepe</t>
   </si>
   <si>
     <t>268/24</t>
   </si>
   <si>
+    <t>https://schroniskochorzow.pl/wp-content/uploads/2024/07/268.png</t>
+  </si>
+  <si>
     <t>Pinio</t>
   </si>
   <si>
@@ -249,12 +321,18 @@
     <t>mały (9,5 kg)</t>
   </si>
   <si>
+    <t>https://schroniskochorzow.pl/wp-content/uploads/2024/07/383-PINIO.png</t>
+  </si>
+  <si>
     <t>Rabus</t>
   </si>
   <si>
     <t>krępy (27 kg)</t>
   </si>
   <si>
+    <t>https://schroniskochorzow.pl/wp-content/uploads/2024/07/70350-Rabus.png</t>
+  </si>
+  <si>
     <t>Rayman</t>
   </si>
   <si>
@@ -264,30 +342,45 @@
     <t>duży (25kg)</t>
   </si>
   <si>
+    <t>https://schroniskochorzow.pl/wp-content/uploads/2024/06/rayman-1.png</t>
+  </si>
+  <si>
     <t>Redi</t>
   </si>
   <si>
     <t>duży (45 kg)</t>
   </si>
   <si>
+    <t>https://schroniskochorzow.pl/wp-content/uploads/2024/07/redi.png</t>
+  </si>
+  <si>
     <t>Scooby-Doo</t>
   </si>
   <si>
     <t>duży (39kg)</t>
   </si>
   <si>
+    <t>https://schroniskochorzow.pl/wp-content/uploads/2024/07/scooby-doo.png</t>
+  </si>
+  <si>
     <t>Tajwan</t>
   </si>
   <si>
     <t>382/23</t>
   </si>
   <si>
+    <t>https://schroniskochorzow.pl/wp-content/uploads/2024/07/382-Tajwan.png</t>
+  </si>
+  <si>
     <t>Teddy</t>
   </si>
   <si>
     <t>olbrzymi (45 kg)</t>
   </si>
   <si>
+    <t>https://schroniskochorzow.pl/wp-content/uploads/2024/07/48497-Teddy.png</t>
+  </si>
+  <si>
     <t>Troy</t>
   </si>
   <si>
@@ -297,6 +390,9 @@
     <t>średni (19 kg)</t>
   </si>
   <si>
+    <t>https://schroniskochorzow.pl/wp-content/uploads/2024/06/troy-1.png</t>
+  </si>
+  <si>
     <t>Ulfik</t>
   </si>
   <si>
@@ -309,27 +405,42 @@
     <t>mały (14kg)</t>
   </si>
   <si>
+    <t>https://schroniskochorzow.pl/wp-content/uploads/2024/07/357.png</t>
+  </si>
+  <si>
     <t>Verka</t>
   </si>
   <si>
     <t>635/20</t>
   </si>
   <si>
+    <t>https://schroniskochorzow.pl/wp-content/uploads/2024/06/verka-1.png</t>
+  </si>
+  <si>
     <t>Wombat</t>
   </si>
   <si>
     <t>288/24</t>
   </si>
   <si>
+    <t>https://schroniskochorzow.pl/wp-content/uploads/2024/07/288-Wombat.png</t>
+  </si>
+  <si>
     <t>Zgrzyt</t>
   </si>
   <si>
     <t>394/19</t>
   </si>
   <si>
+    <t>https://schroniskochorzow.pl/wp-content/uploads/2024/06/zgrzyt1.png</t>
+  </si>
+  <si>
     <t>Zuch</t>
   </si>
   <si>
+    <t>https://schroniskochorzow.pl/wp-content/uploads/2024/07/zuch-1.png</t>
+  </si>
+  <si>
     <t>Testy</t>
   </si>
   <si>
@@ -339,19 +450,25 @@
     <t>164/24</t>
   </si>
   <si>
-    <t>ok. 10 lat</t>
+    <t>ok. 10 latTest FIV/FELV (-)</t>
   </si>
   <si>
     <t>Test FIV/FELV (-)</t>
   </si>
   <si>
+    <t>https://schroniskochorzow.pl/wp-content/uploads/2024/07/cintra-1.png</t>
+  </si>
+  <si>
     <t>Dikens</t>
   </si>
   <si>
     <t>186/24</t>
   </si>
   <si>
-    <t>ok. 5 lat</t>
+    <t>ok. 5 latTest FIV/FELV (-)</t>
+  </si>
+  <si>
+    <t>https://schroniskochorzow.pl/wp-content/uploads/2024/07/dikens-1.png</t>
   </si>
   <si>
     <t>Fifa</t>
@@ -360,7 +477,10 @@
     <t>306/24</t>
   </si>
   <si>
-    <t>ok. 7 tyg.</t>
+    <t>ok. 7 tyg.Test FIV/FELV (-)</t>
+  </si>
+  <si>
+    <t>https://schroniskochorzow.pl/wp-content/uploads/2024/07/306-fifa.png</t>
   </si>
   <si>
     <t>Gienia</t>
@@ -369,13 +489,19 @@
     <t>72/24</t>
   </si>
   <si>
+    <t>https://schroniskochorzow.pl/wp-content/uploads/2024/07/gienia-2.png</t>
+  </si>
+  <si>
     <t>Gryzelda</t>
   </si>
   <si>
     <t>294/24</t>
   </si>
   <si>
-    <t>ok. 4 lat</t>
+    <t>ok. 4 lataTest FIV/FELV (-)</t>
+  </si>
+  <si>
+    <t>https://schroniskochorzow.pl/wp-content/uploads/2024/07/294.png</t>
   </si>
   <si>
     <t>Grzechotka</t>
@@ -384,7 +510,10 @@
     <t>302/24</t>
   </si>
   <si>
-    <t>ok. 10 mies.</t>
+    <t>ok. 10 mies.Test FIV/FELV (-)</t>
+  </si>
+  <si>
+    <t>https://schroniskochorzow.pl/wp-content/uploads/2024/07/302-2.png</t>
   </si>
   <si>
     <t>Halincia</t>
@@ -393,95 +522,231 @@
     <t>322/24</t>
   </si>
   <si>
+    <t>https://schroniskochorzow.pl/wp-content/uploads/2024/07/322-halincia.png</t>
+  </si>
+  <si>
     <t>Helenka</t>
   </si>
   <si>
     <t>279/24</t>
   </si>
   <si>
+    <t>ok. 7 tyg.Test FIV (+) / FELV (-)</t>
+  </si>
+  <si>
     <t>Test FIV (+) / FELV (-)</t>
   </si>
   <si>
+    <t>https://schroniskochorzow.pl/wp-content/uploads/2024/07/279.png</t>
+  </si>
+  <si>
     <t>Henryczka</t>
   </si>
   <si>
     <t>282/24</t>
   </si>
   <si>
+    <t>https://schroniskochorzow.pl/wp-content/uploads/2024/07/282.png</t>
+  </si>
+  <si>
+    <t>Hiacynta</t>
+  </si>
+  <si>
+    <t>281/24</t>
+  </si>
+  <si>
+    <t>https://schroniskochorzow.pl/wp-content/uploads/2024/07/281.png</t>
+  </si>
+  <si>
+    <t>Kiara</t>
+  </si>
+  <si>
+    <t>374/24</t>
+  </si>
+  <si>
+    <t>ok. 11 tyg.Test FIV/FELV (?)</t>
+  </si>
+  <si>
+    <t>Test FIV/FELV (?)</t>
+  </si>
+  <si>
+    <t>https://schroniskochorzow.pl/wp-content/uploads/2024/08/374.png</t>
+  </si>
+  <si>
+    <t>Kinio</t>
+  </si>
+  <si>
+    <t>349/24</t>
+  </si>
+  <si>
+    <t>ok. 10 tyg.Test FIV/FELV (-)</t>
+  </si>
+  <si>
+    <t>https://schroniskochorzow.pl/wp-content/uploads/2024/07/349-1.png</t>
+  </si>
+  <si>
+    <t>Kiwi</t>
+  </si>
+  <si>
+    <t>248/24</t>
+  </si>
+  <si>
+    <t>ok. 6 tyg.Test FIV/FELV (?)</t>
+  </si>
+  <si>
+    <t>https://schroniskochorzow.pl/wp-content/uploads/2024/08/248-kiwi.png</t>
+  </si>
+  <si>
+    <t>Klara</t>
+  </si>
+  <si>
+    <t>230/24</t>
+  </si>
+  <si>
+    <t>https://schroniskochorzow.pl/wp-content/uploads/2024/07/klara-1.png</t>
+  </si>
+  <si>
+    <t>Klementyna</t>
+  </si>
+  <si>
+    <t>88/24</t>
+  </si>
+  <si>
+    <t>ok. 2 lataTest FIV/FELV (-)</t>
+  </si>
+  <si>
+    <t>https://schroniskochorzow.pl/wp-content/uploads/2024/07/klementyna-1.png</t>
+  </si>
+  <si>
+    <t>Koala</t>
+  </si>
+  <si>
+    <t>172/24</t>
+  </si>
+  <si>
+    <t>ok. 8 latTest FIV/FELV (-)</t>
+  </si>
+  <si>
+    <t>https://schroniskochorzow.pl/wp-content/uploads/2024/07/koala-3.png</t>
+  </si>
+  <si>
+    <t>Konwalia</t>
+  </si>
+  <si>
+    <t>338/24</t>
+  </si>
+  <si>
+    <t>https://schroniskochorzow.pl/wp-content/uploads/2024/07/338-Konwalia-1.png</t>
+  </si>
+  <si>
+    <t>Koperek</t>
+  </si>
+  <si>
+    <t>340/24</t>
+  </si>
+  <si>
+    <t>https://schroniskochorzow.pl/wp-content/uploads/2024/07/340-Koperek.png</t>
+  </si>
+  <si>
+    <t>Krokus</t>
+  </si>
+  <si>
+    <t>339/24</t>
+  </si>
+  <si>
+    <t>https://schroniskochorzow.pl/wp-content/uploads/2024/07/339-Kroton-1.png</t>
+  </si>
+  <si>
+    <t>Mosiek</t>
+  </si>
+  <si>
+    <t>226/24</t>
+  </si>
+  <si>
+    <t>ok. 8 tyg.Test FIV/FELV (?)</t>
+  </si>
+  <si>
+    <t>https://schroniskochorzow.pl/wp-content/uploads/2024/08/226-mosiek.png</t>
+  </si>
+  <si>
+    <t>Piramidka</t>
+  </si>
+  <si>
+    <t>120/24</t>
+  </si>
+  <si>
+    <t>https://schroniskochorzow.pl/wp-content/uploads/2024/07/piramidka-2.png</t>
+  </si>
+  <si>
+    <t>Pysia</t>
+  </si>
+  <si>
+    <t>273/24</t>
+  </si>
+  <si>
+    <t>ok. 7 tyg.Test FIV/FELV (?)</t>
+  </si>
+  <si>
+    <t>https://schroniskochorzow.pl/wp-content/uploads/2024/08/273-pysia.png</t>
+  </si>
+  <si>
+    <t>Rafa</t>
+  </si>
+  <si>
+    <t>307/24</t>
+  </si>
+  <si>
+    <t>https://schroniskochorzow.pl/wp-content/uploads/2024/07/307-rafa.png</t>
+  </si>
+  <si>
+    <t>Shakira</t>
+  </si>
+  <si>
+    <t>290/24</t>
+  </si>
+  <si>
+    <t>ok. 4 mies.Test FIV (+) / FELV (-)</t>
+  </si>
+  <si>
+    <t>https://schroniskochorzow.pl/wp-content/uploads/2024/07/289-2.png</t>
+  </si>
+  <si>
+    <t>Szila</t>
+  </si>
+  <si>
+    <t>157/24</t>
+  </si>
+  <si>
+    <t>ok. 1,5 rokuTest FIV/FELV (-)</t>
+  </si>
+  <si>
+    <t>https://schroniskochorzow.pl/wp-content/uploads/2024/07/szila-1.png</t>
+  </si>
+  <si>
     <t>Kwarantanna do:</t>
   </si>
   <si>
     <t>Znaleziona</t>
-  </si>
-  <si>
-    <t>14.08.2024</t>
-  </si>
-  <si>
-    <t>4,5 roku</t>
-  </si>
-  <si>
-    <t>Chorzów</t>
-  </si>
-  <si>
-    <t>3 lata</t>
-  </si>
-  <si>
-    <t>Koziegłowy</t>
-  </si>
-  <si>
-    <t>387/24</t>
-  </si>
-  <si>
-    <t>12.08.2024</t>
-  </si>
-  <si>
-    <t>386/24</t>
-  </si>
-  <si>
-    <t>4 lata</t>
-  </si>
-  <si>
-    <t>Siemianowice Śląskie</t>
-  </si>
-  <si>
-    <t>385/24</t>
-  </si>
-  <si>
-    <t>7 lat</t>
-  </si>
-  <si>
-    <t>Dąbrowa Górnicza</t>
-  </si>
-  <si>
-    <t>383/24</t>
-  </si>
-  <si>
-    <t>1 rok</t>
-  </si>
-  <si>
-    <t>382/24</t>
-  </si>
-  <si>
-    <t>3 miesiące</t>
-  </si>
-  <si>
-    <t>Świętochłowice</t>
-  </si>
-  <si>
-    <t>381/24</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -501,13 +766,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -800,13 +1071,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E37"/>
+  <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -822,633 +1093,782 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2">
         <v>58793</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+        <v>9</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B3">
         <v>29619</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+        <v>13</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B4">
         <v>55970</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+        <v>18</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D5" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="E5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
+        <v>23</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" t="s">
         <v>22</v>
       </c>
-      <c r="E6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" t="s">
-        <v>18</v>
-      </c>
       <c r="E7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
+        <v>32</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="B8" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="C8" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D8" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="E8" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
+        <v>36</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="B9" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="C9" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="D9" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="E9" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
+        <v>42</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="B10">
         <v>43414</v>
       </c>
       <c r="C10" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D10" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E10" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
+        <v>45</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="B11">
         <v>78878</v>
       </c>
       <c r="C11" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D11" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="E11" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
+        <v>48</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="B12">
         <v>34743</v>
       </c>
       <c r="C12" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D12" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E12" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
+        <v>51</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="B13">
         <v>57239</v>
       </c>
       <c r="C13" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D13" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="E13" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
+        <v>55</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="B14" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="C14" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D14" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="E14" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
+        <v>59</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>47</v>
+        <v>61</v>
       </c>
       <c r="B15" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="C15" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D15" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
       <c r="E15" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
+        <v>64</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="B16">
         <v>12822</v>
       </c>
       <c r="C16" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D16" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="E16" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
+        <v>68</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>54</v>
+        <v>70</v>
       </c>
       <c r="B17" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="C17" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D17" t="s">
-        <v>56</v>
+        <v>72</v>
       </c>
       <c r="E17" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
+        <v>73</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>58</v>
+        <v>75</v>
       </c>
       <c r="B18">
         <v>56446</v>
       </c>
       <c r="C18" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D18" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="E18" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
+        <v>48</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="B19">
         <v>30418</v>
       </c>
       <c r="C19" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D19" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="E19" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
+        <v>78</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>61</v>
+        <v>80</v>
       </c>
       <c r="B20">
         <v>59398</v>
       </c>
       <c r="C20" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D20" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="E20" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
+        <v>81</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>63</v>
+        <v>83</v>
       </c>
       <c r="B21">
         <v>54805</v>
       </c>
       <c r="C21" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D21" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E21" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
+        <v>84</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
       <c r="A22" t="s">
-        <v>65</v>
+        <v>86</v>
       </c>
       <c r="B22" t="s">
-        <v>66</v>
+        <v>87</v>
       </c>
       <c r="C22" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D22" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="E22" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
+        <v>9</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
       <c r="A23" t="s">
-        <v>67</v>
+        <v>89</v>
       </c>
       <c r="B23" t="s">
-        <v>68</v>
+        <v>90</v>
       </c>
       <c r="C23" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D23" t="s">
-        <v>69</v>
+        <v>91</v>
       </c>
       <c r="E23" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
+        <v>92</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
       <c r="A24" t="s">
-        <v>71</v>
+        <v>94</v>
       </c>
       <c r="B24" t="s">
-        <v>72</v>
+        <v>95</v>
       </c>
       <c r="C24" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D24" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="E24" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
+        <v>84</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
       <c r="A25" t="s">
-        <v>73</v>
+        <v>97</v>
       </c>
       <c r="B25" t="s">
-        <v>74</v>
+        <v>98</v>
       </c>
       <c r="C25" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D25" t="s">
-        <v>75</v>
+        <v>99</v>
       </c>
       <c r="E25" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
+        <v>100</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
       <c r="A26" t="s">
-        <v>77</v>
+        <v>102</v>
       </c>
       <c r="B26">
         <v>70350</v>
       </c>
       <c r="C26" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D26" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E26" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
+        <v>103</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
       <c r="A27" t="s">
-        <v>79</v>
+        <v>105</v>
       </c>
       <c r="B27" t="s">
-        <v>80</v>
+        <v>106</v>
       </c>
       <c r="C27" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D27" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E27" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5">
+        <v>107</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
       <c r="A28" t="s">
-        <v>82</v>
+        <v>109</v>
       </c>
       <c r="B28">
         <v>45918</v>
       </c>
       <c r="C28" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D28" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E28" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
+        <v>110</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
       <c r="A29" t="s">
-        <v>84</v>
+        <v>112</v>
       </c>
       <c r="B29">
         <v>57049</v>
       </c>
       <c r="C29" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D29" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E29" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5">
+        <v>113</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
       <c r="A30" t="s">
-        <v>86</v>
+        <v>115</v>
       </c>
       <c r="B30" t="s">
-        <v>87</v>
+        <v>116</v>
       </c>
       <c r="C30" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D30" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E30" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5">
+        <v>45</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
       <c r="A31" t="s">
-        <v>88</v>
+        <v>118</v>
       </c>
       <c r="B31">
         <v>48497</v>
       </c>
       <c r="C31" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D31" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="E31" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5">
+        <v>119</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
       <c r="A32" t="s">
-        <v>90</v>
+        <v>121</v>
       </c>
       <c r="B32" t="s">
+        <v>122</v>
+      </c>
+      <c r="C32" t="s">
+        <v>16</v>
+      </c>
+      <c r="D32" t="s">
+        <v>41</v>
+      </c>
+      <c r="E32" t="s">
+        <v>123</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" t="s">
+        <v>125</v>
+      </c>
+      <c r="B33" t="s">
+        <v>126</v>
+      </c>
+      <c r="C33" t="s">
+        <v>16</v>
+      </c>
+      <c r="D33" t="s">
+        <v>127</v>
+      </c>
+      <c r="E33" t="s">
+        <v>128</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" t="s">
+        <v>130</v>
+      </c>
+      <c r="B34" t="s">
+        <v>131</v>
+      </c>
+      <c r="C34" t="s">
+        <v>7</v>
+      </c>
+      <c r="D34" t="s">
         <v>91</v>
       </c>
-      <c r="C32" t="s">
-        <v>13</v>
-      </c>
-      <c r="D32" t="s">
-        <v>33</v>
-      </c>
-      <c r="E32" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5">
-      <c r="A33" t="s">
-        <v>93</v>
-      </c>
-      <c r="B33" t="s">
-        <v>94</v>
-      </c>
-      <c r="C33" t="s">
-        <v>13</v>
-      </c>
-      <c r="D33" t="s">
-        <v>95</v>
-      </c>
-      <c r="E33" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5">
-      <c r="A34" t="s">
-        <v>97</v>
-      </c>
-      <c r="B34" t="s">
-        <v>98</v>
-      </c>
-      <c r="C34" t="s">
-        <v>6</v>
-      </c>
-      <c r="D34" t="s">
-        <v>69</v>
-      </c>
       <c r="E34" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5">
+        <v>28</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
       <c r="A35" t="s">
+        <v>133</v>
+      </c>
+      <c r="B35" t="s">
+        <v>134</v>
+      </c>
+      <c r="C35" t="s">
+        <v>16</v>
+      </c>
+      <c r="D35" t="s">
         <v>99</v>
       </c>
-      <c r="B35" t="s">
-        <v>100</v>
-      </c>
-      <c r="C35" t="s">
-        <v>13</v>
-      </c>
-      <c r="D35" t="s">
-        <v>75</v>
-      </c>
       <c r="E35" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5">
+        <v>123</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
       <c r="A36" t="s">
-        <v>101</v>
+        <v>136</v>
       </c>
       <c r="B36" t="s">
-        <v>102</v>
+        <v>137</v>
       </c>
       <c r="C36" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D36" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="E36" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5">
+        <v>9</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
       <c r="A37" t="s">
-        <v>103</v>
+        <v>139</v>
       </c>
       <c r="B37">
         <v>59588</v>
       </c>
       <c r="C37" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D37" t="s">
-        <v>75</v>
+        <v>99</v>
       </c>
       <c r="E37" t="s">
-        <v>40</v>
+        <v>51</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>140</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F2" r:id="rId1"/>
+    <hyperlink ref="F3" r:id="rId2"/>
+    <hyperlink ref="F4" r:id="rId3"/>
+    <hyperlink ref="F5" r:id="rId4"/>
+    <hyperlink ref="F6" r:id="rId5"/>
+    <hyperlink ref="F7" r:id="rId6"/>
+    <hyperlink ref="F8" r:id="rId7"/>
+    <hyperlink ref="F9" r:id="rId8"/>
+    <hyperlink ref="F10" r:id="rId9"/>
+    <hyperlink ref="F11" r:id="rId10"/>
+    <hyperlink ref="F12" r:id="rId11"/>
+    <hyperlink ref="F13" r:id="rId12"/>
+    <hyperlink ref="F14" r:id="rId13"/>
+    <hyperlink ref="F15" r:id="rId14"/>
+    <hyperlink ref="F16" r:id="rId15"/>
+    <hyperlink ref="F17" r:id="rId16"/>
+    <hyperlink ref="F18" r:id="rId17"/>
+    <hyperlink ref="F19" r:id="rId18"/>
+    <hyperlink ref="F20" r:id="rId19"/>
+    <hyperlink ref="F21" r:id="rId20"/>
+    <hyperlink ref="F22" r:id="rId21"/>
+    <hyperlink ref="F23" r:id="rId22"/>
+    <hyperlink ref="F24" r:id="rId23"/>
+    <hyperlink ref="F25" r:id="rId24"/>
+    <hyperlink ref="F26" r:id="rId25"/>
+    <hyperlink ref="F27" r:id="rId26"/>
+    <hyperlink ref="F28" r:id="rId27"/>
+    <hyperlink ref="F29" r:id="rId28"/>
+    <hyperlink ref="F30" r:id="rId29"/>
+    <hyperlink ref="F31" r:id="rId30"/>
+    <hyperlink ref="F32" r:id="rId31"/>
+    <hyperlink ref="F33" r:id="rId32"/>
+    <hyperlink ref="F34" r:id="rId33"/>
+    <hyperlink ref="F35" r:id="rId34"/>
+    <hyperlink ref="F36" r:id="rId35"/>
+    <hyperlink ref="F37" r:id="rId36"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1462,181 +1882,558 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
+        <v>141</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>105</v>
+        <v>142</v>
       </c>
       <c r="B2" t="s">
-        <v>106</v>
+        <v>143</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>107</v>
+        <v>144</v>
       </c>
       <c r="E2" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+        <v>145</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>109</v>
+        <v>147</v>
       </c>
       <c r="B3" t="s">
-        <v>110</v>
+        <v>148</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>111</v>
+        <v>149</v>
       </c>
       <c r="E3" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+        <v>145</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>112</v>
+        <v>151</v>
       </c>
       <c r="B4" t="s">
-        <v>113</v>
+        <v>152</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>114</v>
+        <v>153</v>
       </c>
       <c r="E4" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+        <v>145</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>115</v>
+        <v>155</v>
       </c>
       <c r="B5" t="s">
-        <v>116</v>
+        <v>156</v>
       </c>
       <c r="C5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D5" t="s">
-        <v>107</v>
+        <v>144</v>
       </c>
       <c r="E5" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
+        <v>145</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>117</v>
+        <v>158</v>
       </c>
       <c r="B6" t="s">
-        <v>118</v>
+        <v>159</v>
       </c>
       <c r="C6" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D6" t="s">
-        <v>119</v>
+        <v>160</v>
       </c>
       <c r="E6" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
+        <v>145</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>120</v>
+        <v>162</v>
       </c>
       <c r="B7" t="s">
-        <v>121</v>
+        <v>163</v>
       </c>
       <c r="C7" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D7" t="s">
-        <v>122</v>
+        <v>164</v>
       </c>
       <c r="E7" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
+        <v>145</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>123</v>
+        <v>166</v>
       </c>
       <c r="B8" t="s">
-        <v>124</v>
+        <v>167</v>
       </c>
       <c r="C8" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>114</v>
+        <v>153</v>
       </c>
       <c r="E8" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
+        <v>145</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>125</v>
+        <v>169</v>
       </c>
       <c r="B9" t="s">
-        <v>126</v>
+        <v>170</v>
       </c>
       <c r="C9" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D9" t="s">
-        <v>114</v>
+        <v>171</v>
       </c>
       <c r="E9" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
+        <v>172</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>128</v>
+        <v>174</v>
       </c>
       <c r="B10" t="s">
-        <v>129</v>
+        <v>175</v>
       </c>
       <c r="C10" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D10" t="s">
-        <v>114</v>
+        <v>171</v>
       </c>
       <c r="E10" t="s">
-        <v>127</v>
+        <v>172</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="s">
+        <v>177</v>
+      </c>
+      <c r="B11" t="s">
+        <v>178</v>
+      </c>
+      <c r="C11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" t="s">
+        <v>171</v>
+      </c>
+      <c r="E11" t="s">
+        <v>172</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" t="s">
+        <v>180</v>
+      </c>
+      <c r="B12" t="s">
+        <v>181</v>
+      </c>
+      <c r="C12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" t="s">
+        <v>182</v>
+      </c>
+      <c r="E12" t="s">
+        <v>183</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" t="s">
+        <v>185</v>
+      </c>
+      <c r="B13" t="s">
+        <v>186</v>
+      </c>
+      <c r="C13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" t="s">
+        <v>187</v>
+      </c>
+      <c r="E13" t="s">
+        <v>145</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" t="s">
+        <v>189</v>
+      </c>
+      <c r="B14" t="s">
+        <v>190</v>
+      </c>
+      <c r="C14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" t="s">
+        <v>191</v>
+      </c>
+      <c r="E14" t="s">
+        <v>183</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" t="s">
+        <v>193</v>
+      </c>
+      <c r="B15" t="s">
+        <v>194</v>
+      </c>
+      <c r="C15" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" t="s">
+        <v>160</v>
+      </c>
+      <c r="E15" t="s">
+        <v>145</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" t="s">
+        <v>196</v>
+      </c>
+      <c r="B16" t="s">
+        <v>197</v>
+      </c>
+      <c r="C16" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" t="s">
+        <v>198</v>
+      </c>
+      <c r="E16" t="s">
+        <v>145</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" t="s">
+        <v>200</v>
+      </c>
+      <c r="B17" t="s">
+        <v>201</v>
+      </c>
+      <c r="C17" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" t="s">
+        <v>202</v>
+      </c>
+      <c r="E17" t="s">
+        <v>145</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" t="s">
+        <v>204</v>
+      </c>
+      <c r="B18" t="s">
+        <v>205</v>
+      </c>
+      <c r="C18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" t="s">
+        <v>153</v>
+      </c>
+      <c r="E18" t="s">
+        <v>145</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" t="s">
+        <v>207</v>
+      </c>
+      <c r="B19" t="s">
+        <v>208</v>
+      </c>
+      <c r="C19" t="s">
+        <v>16</v>
+      </c>
+      <c r="D19" t="s">
+        <v>153</v>
+      </c>
+      <c r="E19" t="s">
+        <v>145</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" t="s">
+        <v>210</v>
+      </c>
+      <c r="B20" t="s">
+        <v>211</v>
+      </c>
+      <c r="C20" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20" t="s">
+        <v>153</v>
+      </c>
+      <c r="E20" t="s">
+        <v>145</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" t="s">
+        <v>213</v>
+      </c>
+      <c r="B21" t="s">
+        <v>214</v>
+      </c>
+      <c r="C21" t="s">
+        <v>16</v>
+      </c>
+      <c r="D21" t="s">
+        <v>215</v>
+      </c>
+      <c r="E21" t="s">
+        <v>183</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" t="s">
+        <v>217</v>
+      </c>
+      <c r="B22" t="s">
+        <v>218</v>
+      </c>
+      <c r="C22" t="s">
+        <v>7</v>
+      </c>
+      <c r="D22" t="s">
+        <v>198</v>
+      </c>
+      <c r="E22" t="s">
+        <v>145</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" t="s">
+        <v>220</v>
+      </c>
+      <c r="B23" t="s">
+        <v>221</v>
+      </c>
+      <c r="C23" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23" t="s">
+        <v>222</v>
+      </c>
+      <c r="E23" t="s">
+        <v>183</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" t="s">
+        <v>224</v>
+      </c>
+      <c r="B24" t="s">
+        <v>225</v>
+      </c>
+      <c r="C24" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24" t="s">
+        <v>153</v>
+      </c>
+      <c r="E24" t="s">
+        <v>145</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" t="s">
+        <v>227</v>
+      </c>
+      <c r="B25" t="s">
+        <v>228</v>
+      </c>
+      <c r="C25" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25" t="s">
+        <v>229</v>
+      </c>
+      <c r="E25" t="s">
+        <v>172</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" t="s">
+        <v>231</v>
+      </c>
+      <c r="B26" t="s">
+        <v>232</v>
+      </c>
+      <c r="C26" t="s">
+        <v>7</v>
+      </c>
+      <c r="D26" t="s">
+        <v>233</v>
+      </c>
+      <c r="E26" t="s">
+        <v>145</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>234</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F2" r:id="rId1"/>
+    <hyperlink ref="F3" r:id="rId2"/>
+    <hyperlink ref="F4" r:id="rId3"/>
+    <hyperlink ref="F5" r:id="rId4"/>
+    <hyperlink ref="F6" r:id="rId5"/>
+    <hyperlink ref="F7" r:id="rId6"/>
+    <hyperlink ref="F8" r:id="rId7"/>
+    <hyperlink ref="F9" r:id="rId8"/>
+    <hyperlink ref="F10" r:id="rId9"/>
+    <hyperlink ref="F11" r:id="rId10"/>
+    <hyperlink ref="F12" r:id="rId11"/>
+    <hyperlink ref="F13" r:id="rId12"/>
+    <hyperlink ref="F14" r:id="rId13"/>
+    <hyperlink ref="F15" r:id="rId14"/>
+    <hyperlink ref="F16" r:id="rId15"/>
+    <hyperlink ref="F17" r:id="rId16"/>
+    <hyperlink ref="F18" r:id="rId17"/>
+    <hyperlink ref="F19" r:id="rId18"/>
+    <hyperlink ref="F20" r:id="rId19"/>
+    <hyperlink ref="F21" r:id="rId20"/>
+    <hyperlink ref="F22" r:id="rId21"/>
+    <hyperlink ref="F23" r:id="rId22"/>
+    <hyperlink ref="F24" r:id="rId23"/>
+    <hyperlink ref="F25" r:id="rId24"/>
+    <hyperlink ref="F26" r:id="rId25"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>130</v>
+        <v>235</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -1645,160 +2442,10 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2">
-        <v>55369</v>
-      </c>
-      <c r="B2" t="s">
-        <v>132</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>133</v>
-      </c>
-      <c r="E2" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3">
-        <v>59825</v>
-      </c>
-      <c r="B3" t="s">
-        <v>132</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" t="s">
-        <v>135</v>
-      </c>
-      <c r="E3" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
-        <v>137</v>
-      </c>
-      <c r="B4" t="s">
-        <v>138</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" t="s">
-        <v>135</v>
-      </c>
-      <c r="E4" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="s">
-        <v>139</v>
-      </c>
-      <c r="B5" t="s">
-        <v>138</v>
-      </c>
-      <c r="C5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" t="s">
-        <v>140</v>
-      </c>
-      <c r="E5" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" t="s">
-        <v>142</v>
-      </c>
-      <c r="B6" t="s">
-        <v>138</v>
-      </c>
-      <c r="C6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" t="s">
-        <v>143</v>
-      </c>
-      <c r="E6" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" t="s">
-        <v>145</v>
-      </c>
-      <c r="B7" t="s">
-        <v>138</v>
-      </c>
-      <c r="C7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" t="s">
-        <v>146</v>
-      </c>
-      <c r="E7" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" t="s">
-        <v>147</v>
-      </c>
-      <c r="B8" t="s">
-        <v>138</v>
-      </c>
-      <c r="C8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" t="s">
-        <v>148</v>
-      </c>
-      <c r="E8" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" t="s">
-        <v>150</v>
-      </c>
-      <c r="B9" t="s">
-        <v>138</v>
-      </c>
-      <c r="C9" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" t="s">
-        <v>135</v>
-      </c>
-      <c r="E9" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10">
-        <v>57698</v>
-      </c>
-      <c r="B10" t="s">
-        <v>138</v>
-      </c>
-      <c r="C10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" t="s">
-        <v>133</v>
-      </c>
-      <c r="E10" t="s">
-        <v>149</v>
+        <v>236</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>